<commit_message>
Start of Teknikbyggnad, added fix for unique Id's. Minor but important change to Teknikbyggnad excel.
</commit_message>
<xml_diff>
--- a/DataMappingExperiments/Testdata/Fln-Blg Teknikbyggnader Detaljlägen.xlsx
+++ b/DataMappingExperiments/Testdata/Fln-Blg Teknikbyggnader Detaljlägen.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\DOK\Anda Nät Anl NJDB NTL\Migrering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fresan\Documents\visual studio 2015\Projects\DataMappingExperiments\DataMappingExperiments\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20955" windowHeight="12375"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20952" windowHeight="12372"/>
   </bookViews>
   <sheets>
     <sheet name="Resultat" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5183" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5183" uniqueCount="468">
   <si>
     <t>Objtypnr</t>
   </si>
@@ -1432,12 +1432,15 @@
   </si>
   <si>
     <t>2017-02-09 12:53</t>
+  </si>
+  <si>
+    <t>Komponent Modell</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1765,81 +1768,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BN137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="BA1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="BJ1" sqref="BJ1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="19.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="21.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="23.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="8.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="20.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="58.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="58.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="9.140625" style="1"/>
-    <col min="62" max="62" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="9.109375" style="1"/>
+    <col min="62" max="62" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="11.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:66" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2024,7 +2027,7 @@
         <v>60</v>
       </c>
       <c r="BJ1" s="5" t="s">
-        <v>29</v>
+        <v>467</v>
       </c>
       <c r="BK1" s="5" t="s">
         <v>61</v>
@@ -2039,7 +2042,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10028</v>
       </c>
@@ -2236,7 +2239,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10028</v>
       </c>
@@ -2433,7 +2436,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10028</v>
       </c>
@@ -2630,7 +2633,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10028</v>
       </c>
@@ -2827,7 +2830,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10028</v>
       </c>
@@ -3024,7 +3027,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10028</v>
       </c>
@@ -3221,7 +3224,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10028</v>
       </c>
@@ -3418,7 +3421,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10028</v>
       </c>
@@ -3615,7 +3618,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10028</v>
       </c>
@@ -3812,7 +3815,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10028</v>
       </c>
@@ -4009,7 +4012,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10028</v>
       </c>
@@ -4206,7 +4209,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10028</v>
       </c>
@@ -4403,7 +4406,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>10028</v>
       </c>
@@ -4600,7 +4603,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10028</v>
       </c>
@@ -4797,7 +4800,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10028</v>
       </c>
@@ -4994,7 +4997,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>10028</v>
       </c>
@@ -5191,7 +5194,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>10028</v>
       </c>
@@ -5388,7 +5391,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>10028</v>
       </c>
@@ -5585,7 +5588,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>10028</v>
       </c>
@@ -5782,7 +5785,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>10028</v>
       </c>
@@ -5979,7 +5982,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>10028</v>
       </c>
@@ -6176,7 +6179,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>10028</v>
       </c>
@@ -6373,7 +6376,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>10028</v>
       </c>
@@ -6570,7 +6573,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>10028</v>
       </c>
@@ -6767,7 +6770,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>10028</v>
       </c>
@@ -6964,7 +6967,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>10028</v>
       </c>
@@ -7161,7 +7164,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>10028</v>
       </c>
@@ -7358,7 +7361,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>10028</v>
       </c>
@@ -7555,7 +7558,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>10028</v>
       </c>
@@ -7752,7 +7755,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>10028</v>
       </c>
@@ -7949,7 +7952,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>10028</v>
       </c>
@@ -8146,7 +8149,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>10028</v>
       </c>
@@ -8340,7 +8343,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>10028</v>
       </c>
@@ -8537,7 +8540,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>10028</v>
       </c>
@@ -8734,7 +8737,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>10028</v>
       </c>
@@ -8931,7 +8934,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>10028</v>
       </c>
@@ -9128,7 +9131,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>10028</v>
       </c>
@@ -9325,7 +9328,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>10028</v>
       </c>
@@ -9519,7 +9522,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>10028</v>
       </c>
@@ -9713,7 +9716,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>10028</v>
       </c>
@@ -9907,7 +9910,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>10028</v>
       </c>
@@ -10104,7 +10107,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>10028</v>
       </c>
@@ -10301,7 +10304,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>10028</v>
       </c>
@@ -10498,7 +10501,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>10028</v>
       </c>
@@ -10695,7 +10698,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>10028</v>
       </c>
@@ -10892,7 +10895,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>10028</v>
       </c>
@@ -11089,7 +11092,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>10028</v>
       </c>
@@ -11283,7 +11286,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="49" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>10028</v>
       </c>
@@ -11480,7 +11483,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>10028</v>
       </c>
@@ -11677,7 +11680,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>10028</v>
       </c>
@@ -11874,7 +11877,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="52" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>10028</v>
       </c>
@@ -12071,7 +12074,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="53" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>10028</v>
       </c>
@@ -12268,7 +12271,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="54" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>10028</v>
       </c>
@@ -12465,7 +12468,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="55" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>10028</v>
       </c>
@@ -12662,7 +12665,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="56" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>10028</v>
       </c>
@@ -12859,7 +12862,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="57" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>10028</v>
       </c>
@@ -13056,7 +13059,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="58" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>10028</v>
       </c>
@@ -13253,7 +13256,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="59" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>10028</v>
       </c>
@@ -13450,7 +13453,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="60" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>10028</v>
       </c>
@@ -13647,7 +13650,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="61" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>10028</v>
       </c>
@@ -13844,7 +13847,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="62" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>10028</v>
       </c>
@@ -14041,7 +14044,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="63" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>10028</v>
       </c>
@@ -14238,7 +14241,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="64" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>10028</v>
       </c>
@@ -14435,7 +14438,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="65" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>10028</v>
       </c>
@@ -14632,7 +14635,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="66" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>10028</v>
       </c>
@@ -14829,7 +14832,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="67" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>10028</v>
       </c>
@@ -15026,7 +15029,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="68" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>10028</v>
       </c>
@@ -15223,7 +15226,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="69" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>10028</v>
       </c>
@@ -15417,7 +15420,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="70" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>10028</v>
       </c>
@@ -15611,7 +15614,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="71" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>10028</v>
       </c>
@@ -15805,7 +15808,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="72" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>10028</v>
       </c>
@@ -15999,7 +16002,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="73" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>10028</v>
       </c>
@@ -16193,7 +16196,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="74" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>10028</v>
       </c>
@@ -16390,7 +16393,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="75" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>10028</v>
       </c>
@@ -16587,7 +16590,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="76" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>10028</v>
       </c>
@@ -16781,7 +16784,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="77" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>10028</v>
       </c>
@@ -16978,7 +16981,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="78" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>10028</v>
       </c>
@@ -17175,7 +17178,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="79" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>10028</v>
       </c>
@@ -17372,7 +17375,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="80" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>10028</v>
       </c>
@@ -17569,7 +17572,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>10028</v>
       </c>
@@ -17766,7 +17769,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>10028</v>
       </c>
@@ -17963,7 +17966,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="83" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>10028</v>
       </c>
@@ -18160,7 +18163,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="84" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>10028</v>
       </c>
@@ -18357,7 +18360,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="85" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>10028</v>
       </c>
@@ -18554,7 +18557,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="86" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>10028</v>
       </c>
@@ -18751,7 +18754,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="87" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>10028</v>
       </c>
@@ -18948,7 +18951,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="88" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>10028</v>
       </c>
@@ -19145,7 +19148,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="89" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>10028</v>
       </c>
@@ -19342,7 +19345,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="90" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>10028</v>
       </c>
@@ -19539,7 +19542,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="91" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>10028</v>
       </c>
@@ -19736,7 +19739,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="92" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>10028</v>
       </c>
@@ -19933,7 +19936,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="93" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>10028</v>
       </c>
@@ -20130,7 +20133,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="94" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>10028</v>
       </c>
@@ -20327,7 +20330,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="95" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>10028</v>
       </c>
@@ -20527,7 +20530,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="96" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>10028</v>
       </c>
@@ -20727,7 +20730,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="97" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>10028</v>
       </c>
@@ -20927,7 +20930,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="98" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>10028</v>
       </c>
@@ -21127,7 +21130,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="99" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>10028</v>
       </c>
@@ -21327,7 +21330,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="100" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>10028</v>
       </c>
@@ -21521,7 +21524,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="101" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>10028</v>
       </c>
@@ -21718,7 +21721,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="102" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>10028</v>
       </c>
@@ -21915,7 +21918,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="103" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>10028</v>
       </c>
@@ -22112,7 +22115,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="104" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>10028</v>
       </c>
@@ -22309,7 +22312,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="105" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>10028</v>
       </c>
@@ -22503,7 +22506,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="106" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>10028</v>
       </c>
@@ -22697,7 +22700,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="107" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>10028</v>
       </c>
@@ -22891,7 +22894,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="108" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>10028</v>
       </c>
@@ -23085,7 +23088,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="109" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>10028</v>
       </c>
@@ -23279,7 +23282,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="110" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>10028</v>
       </c>
@@ -23473,7 +23476,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="111" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>10028</v>
       </c>
@@ -23667,7 +23670,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="112" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>10028</v>
       </c>
@@ -23861,7 +23864,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="113" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>10028</v>
       </c>
@@ -24058,7 +24061,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="114" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>10028</v>
       </c>
@@ -24255,7 +24258,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="115" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>10028</v>
       </c>
@@ -24452,7 +24455,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="116" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>10028</v>
       </c>
@@ -24646,7 +24649,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="117" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>10028</v>
       </c>
@@ -24840,7 +24843,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="118" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>10028</v>
       </c>
@@ -25037,7 +25040,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="119" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>10028</v>
       </c>
@@ -25234,7 +25237,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="120" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>10028</v>
       </c>
@@ -25431,7 +25434,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="121" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>10028</v>
       </c>
@@ -25628,7 +25631,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="122" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>10028</v>
       </c>
@@ -25822,7 +25825,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="123" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>10028</v>
       </c>
@@ -26019,7 +26022,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="124" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>10028</v>
       </c>
@@ -26216,7 +26219,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="125" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>10028</v>
       </c>
@@ -26410,7 +26413,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="126" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>10028</v>
       </c>
@@ -26607,7 +26610,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="127" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>10028</v>
       </c>
@@ -26804,7 +26807,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="128" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>10028</v>
       </c>
@@ -26998,7 +27001,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="129" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>10028</v>
       </c>
@@ -27192,7 +27195,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="130" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>10028</v>
       </c>
@@ -27386,7 +27389,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="131" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>10028</v>
       </c>
@@ -27580,7 +27583,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="132" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>10028</v>
       </c>
@@ -27777,7 +27780,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="133" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>10028</v>
       </c>
@@ -27974,7 +27977,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="134" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>10028</v>
       </c>
@@ -28171,7 +28174,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="135" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>10028</v>
       </c>
@@ -28368,7 +28371,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="136" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>10028</v>
       </c>
@@ -28565,7 +28568,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="137" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>10028</v>
       </c>
@@ -28778,14 +28781,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>457</v>
       </c>
@@ -28805,7 +28808,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>79</v>
       </c>
@@ -28825,7 +28828,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>458</v>
       </c>
@@ -28845,7 +28848,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>459</v>
       </c>
@@ -28865,7 +28868,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>459</v>
       </c>
@@ -28885,7 +28888,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>459</v>
       </c>
@@ -28905,7 +28908,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>459</v>
       </c>
@@ -28925,7 +28928,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>459</v>
       </c>
@@ -28945,7 +28948,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>459</v>
       </c>
@@ -28965,7 +28968,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>459</v>
       </c>
@@ -28985,7 +28988,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>459</v>
       </c>
@@ -29005,7 +29008,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>459</v>
       </c>
@@ -29025,7 +29028,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>459</v>
       </c>
@@ -29045,7 +29048,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>459</v>
       </c>
@@ -29065,7 +29068,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>459</v>
       </c>
@@ -29085,7 +29088,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>459</v>
       </c>
@@ -29105,7 +29108,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>459</v>
       </c>
@@ -29125,7 +29128,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>459</v>
       </c>
@@ -29145,7 +29148,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>459</v>
       </c>
@@ -29165,7 +29168,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>459</v>
       </c>
@@ -29185,7 +29188,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>459</v>
       </c>
@@ -29205,7 +29208,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>459</v>
       </c>
@@ -29225,7 +29228,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>459</v>
       </c>
@@ -29245,7 +29248,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>459</v>
       </c>
@@ -29265,7 +29268,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>459</v>
       </c>
@@ -29285,7 +29288,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>459</v>
       </c>
@@ -29305,7 +29308,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>459</v>
       </c>
@@ -29325,7 +29328,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>459</v>
       </c>
@@ -29345,7 +29348,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>459</v>
       </c>
@@ -29365,7 +29368,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>459</v>
       </c>
@@ -29385,7 +29388,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>459</v>
       </c>
@@ -29405,7 +29408,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>459</v>
       </c>
@@ -29425,7 +29428,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>459</v>
       </c>
@@ -29445,7 +29448,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>459</v>
       </c>
@@ -29465,7 +29468,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>459</v>
       </c>
@@ -29485,7 +29488,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>459</v>
       </c>
@@ -29505,7 +29508,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>459</v>
       </c>
@@ -29525,7 +29528,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>459</v>
       </c>
@@ -29545,7 +29548,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>459</v>
       </c>
@@ -29565,7 +29568,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>459</v>
       </c>
@@ -29585,7 +29588,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>79</v>
       </c>
@@ -29605,7 +29608,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>460</v>
       </c>
@@ -29625,7 +29628,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>84</v>
       </c>
@@ -29645,7 +29648,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>67</v>
       </c>
@@ -29665,7 +29668,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>465</v>
       </c>
@@ -29688,7 +29691,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -29700,7 +29703,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -29712,7 +29715,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated for the new input files
</commit_message>
<xml_diff>
--- a/DataMappingExperiments/Testdata/Fln-Blg Teknikbyggnader Detaljlägen.xlsx
+++ b/DataMappingExperiments/Testdata/Fln-Blg Teknikbyggnader Detaljlägen.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fresan\Documents\visual studio 2015\Projects\DataMappingExperiments\DataMappingExperiments\Testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fresan\Documents\Visual Studio 2015\Projects\DataMappingExperiments\DataMappingExperiments\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1768,7 +1768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BN137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BA1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="BJ1" sqref="BJ1"/>
     </sheetView>

</xml_diff>